<commit_message>
unet and multi modal final
</commit_message>
<xml_diff>
--- a/cityscapes/unet_classification_report.xlsx
+++ b/cityscapes/unet_classification_report.xlsx
@@ -462,16 +462,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.9106372823753113</v>
+        <v>0.9111723536751646</v>
       </c>
       <c r="C2" t="n">
-        <v>0.592990618968124</v>
+        <v>0.5924365164188126</v>
       </c>
       <c r="D2" t="n">
-        <v>0.7182619652757399</v>
+        <v>0.718021535793023</v>
       </c>
       <c r="E2" t="n">
-        <v>2400269</v>
+        <v>2392469</v>
       </c>
     </row>
     <row r="3">
@@ -481,16 +481,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.8231442390529604</v>
+        <v>0.8232512685468957</v>
       </c>
       <c r="C3" t="n">
-        <v>0.9463093299953514</v>
+        <v>0.9464225403740646</v>
       </c>
       <c r="D3" t="n">
-        <v>0.8804402522601286</v>
+        <v>0.8805504754793186</v>
       </c>
       <c r="E3" t="n">
-        <v>6210539</v>
+        <v>6176366</v>
       </c>
     </row>
     <row r="4">
@@ -500,16 +500,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.4372008955365322</v>
+        <v>0.4366230743875172</v>
       </c>
       <c r="C4" t="n">
-        <v>0.4151660589244369</v>
+        <v>0.416124084407222</v>
       </c>
       <c r="D4" t="n">
-        <v>0.4258986620918986</v>
+        <v>0.4261271941787977</v>
       </c>
       <c r="E4" t="n">
-        <v>1066790</v>
+        <v>1056829</v>
       </c>
     </row>
     <row r="5">
@@ -519,16 +519,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.6958515391512773</v>
+        <v>0.6955661618336961</v>
       </c>
       <c r="C5" t="n">
-        <v>0.7712953874460624</v>
+        <v>0.7713393947968766</v>
       </c>
       <c r="D5" t="n">
-        <v>0.7316337208835297</v>
+        <v>0.7314957392926512</v>
       </c>
       <c r="E5" t="n">
-        <v>3896865</v>
+        <v>3873212</v>
       </c>
     </row>
     <row r="6">
@@ -547,7 +547,7 @@
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>124204</v>
+        <v>123974</v>
       </c>
     </row>
     <row r="7">
@@ -566,7 +566,7 @@
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>169345</v>
+        <v>168578</v>
       </c>
     </row>
     <row r="8">
@@ -585,7 +585,7 @@
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>215210</v>
+        <v>214004</v>
       </c>
     </row>
     <row r="9">
@@ -604,7 +604,7 @@
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>37082</v>
+        <v>36592</v>
       </c>
     </row>
     <row r="10">
@@ -623,7 +623,7 @@
         <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>100407</v>
+        <v>100191</v>
       </c>
     </row>
     <row r="11">
@@ -633,16 +633,16 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.6822634741290393</v>
+        <v>0.6826874078569123</v>
       </c>
       <c r="C11" t="n">
-        <v>0.7703970489887988</v>
+        <v>0.7708375349227572</v>
       </c>
       <c r="D11" t="n">
-        <v>0.7236567095163229</v>
+        <v>0.7240895055971512</v>
       </c>
       <c r="E11" t="n">
-        <v>2742382</v>
+        <v>2732101</v>
       </c>
     </row>
     <row r="12">
@@ -661,7 +661,7 @@
         <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>203209</v>
+        <v>201385</v>
       </c>
     </row>
     <row r="13">
@@ -671,16 +671,16 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.8095560993474067</v>
+        <v>0.8095354264863391</v>
       </c>
       <c r="C13" t="n">
-        <v>0.922929735216188</v>
+        <v>0.922536457148634</v>
       </c>
       <c r="D13" t="n">
-        <v>0.8625333396755409</v>
+        <v>0.8623498266361862</v>
       </c>
       <c r="E13" t="n">
-        <v>677836</v>
+        <v>672639</v>
       </c>
     </row>
     <row r="14">
@@ -699,7 +699,7 @@
         <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>236267</v>
+        <v>236220</v>
       </c>
     </row>
     <row r="15">
@@ -728,16 +728,16 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.5908575663090203</v>
+        <v>0.5916600215120491</v>
       </c>
       <c r="C16" t="n">
-        <v>0.7885365489797731</v>
+        <v>0.789285879206915</v>
       </c>
       <c r="D16" t="n">
-        <v>0.6755325125892069</v>
+        <v>0.6763319258597904</v>
       </c>
       <c r="E16" t="n">
-        <v>1193166</v>
+        <v>1191045</v>
       </c>
     </row>
     <row r="17">
@@ -756,7 +756,7 @@
         <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>40316</v>
+        <v>40011</v>
       </c>
     </row>
     <row r="18">
@@ -813,7 +813,7 @@
         <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>14642</v>
+        <v>14625</v>
       </c>
     </row>
     <row r="21">
@@ -832,7 +832,7 @@
         <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>75232</v>
+        <v>75216</v>
       </c>
     </row>
     <row r="22">
@@ -842,16 +842,16 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.7400194697019433</v>
+        <v>0.7400917878022065</v>
       </c>
       <c r="C22" t="n">
-        <v>0.7400194697019433</v>
+        <v>0.7400917878022065</v>
       </c>
       <c r="D22" t="n">
-        <v>0.7400194697019433</v>
+        <v>0.7400917878022065</v>
       </c>
       <c r="E22" t="n">
-        <v>0.7400194697019433</v>
+        <v>0.7400917878022065</v>
       </c>
     </row>
     <row r="23">
@@ -861,16 +861,16 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.2474755547950774</v>
+        <v>0.2475247857149287</v>
       </c>
       <c r="C23" t="n">
-        <v>0.2603812364259367</v>
+        <v>0.2604491203637641</v>
       </c>
       <c r="D23" t="n">
-        <v>0.2508978581146184</v>
+        <v>0.2509483101418459</v>
       </c>
       <c r="E23" t="n">
-        <v>19496960</v>
+        <v>19398656</v>
       </c>
     </row>
     <row r="24">
@@ -880,16 +880,16 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.6975830789870042</v>
+        <v>0.6977057403346049</v>
       </c>
       <c r="C24" t="n">
-        <v>0.7400194697019433</v>
+        <v>0.7400917878022065</v>
       </c>
       <c r="D24" t="n">
-        <v>0.7115301275445368</v>
+        <v>0.7115908175097977</v>
       </c>
       <c r="E24" t="n">
-        <v>19496960</v>
+        <v>19398656</v>
       </c>
     </row>
   </sheetData>

</xml_diff>